<commit_message>
AFDP-7334 Admin Module - Holiday Schedule Misspelling
</commit_message>
<xml_diff>
--- a/acm/rules/drools-ocr-business-process-rules.xlsx
+++ b/acm/rules/drools-ocr-business-process-rules.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\ArkCase\acm-tool-integrations\acm-ocr\src\main\resources\rules\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ana.serafimoska\.arkcase\acm\rules\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C0CDD49-8B48-4A1E-AA47-243FF53DBA0B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3DD3CD4-887E-42B6-8864-0980A9F7E5BA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="997" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -179,9 +179,6 @@
     <t>eval(evalSpring("$param", $model))</t>
   </si>
   <si>
-    <t>OCRWrokflow</t>
-  </si>
-  <si>
     <t>$model: OCRBusinessProcessModel</t>
   </si>
   <si>
@@ -201,6 +198,9 @@
   </si>
   <si>
     <t>com.armedia.acm.ocr.model.OCRBusinessProcessModel</t>
+  </si>
+  <si>
+    <t>OCRWorkflow</t>
   </si>
 </sst>
 </file>
@@ -1091,8 +1091,8 @@
   </sheetPr>
   <dimension ref="A1:G18"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+    <sheetView tabSelected="1" topLeftCell="A9" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1123,7 +1123,7 @@
         <v>0</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E2" s="1"/>
       <c r="F2" s="1"/>
@@ -1136,7 +1136,7 @@
         <v>1</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E3" s="1"/>
       <c r="F3" s="1"/>
@@ -1228,7 +1228,7 @@
       <c r="A12" s="2"/>
       <c r="B12" s="2"/>
       <c r="C12" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D12" s="3"/>
       <c r="E12" s="3"/>
@@ -1250,7 +1250,7 @@
       <c r="A14" s="2"/>
       <c r="B14" s="2"/>
       <c r="C14" s="5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D14" s="9"/>
       <c r="E14" s="9"/>
@@ -1276,7 +1276,7 @@
         <v>7</v>
       </c>
       <c r="C16" s="14" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D16" s="15" t="s">
         <v>8</v>
@@ -1288,7 +1288,7 @@
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="16"/>
       <c r="B17" s="17" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C17" s="18" t="s">
         <v>19</v>
@@ -1297,7 +1297,7 @@
         <v>3</v>
       </c>
       <c r="E17" s="19" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
       <c r="F17" s="19"/>
       <c r="G17" s="19"/>
@@ -1305,7 +1305,7 @@
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="16"/>
       <c r="B18" s="17" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C18" s="18" t="s">
         <v>20</v>
@@ -1314,7 +1314,7 @@
         <v>3</v>
       </c>
       <c r="E18" s="19" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
       <c r="F18" s="19"/>
       <c r="G18" s="19"/>

</xml_diff>

<commit_message>
AFDP-7308 Combine Transcribe and OCR processing into a single media processing module
</commit_message>
<xml_diff>
--- a/acm/rules/drools-ocr-business-process-rules.xlsx
+++ b/acm/rules/drools-ocr-business-process-rules.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ana.serafimoska\.arkcase\acm\rules\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vladimir.cherepnalko\.arkcase\acm\rules\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3DD3CD4-887E-42B6-8864-0980A9F7E5BA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3877ADAB-A4F3-4005-8297-F3BD2E86AC5D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="997" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -179,9 +179,6 @@
     <t>eval(evalSpring("$param", $model))</t>
   </si>
   <si>
-    <t>$model: OCRBusinessProcessModel</t>
-  </si>
-  <si>
     <t>Automatic OCR</t>
   </si>
   <si>
@@ -197,10 +194,13 @@
     <t>OCR Workflow Rules</t>
   </si>
   <si>
-    <t>com.armedia.acm.ocr.model.OCRBusinessProcessModel</t>
-  </si>
-  <si>
-    <t>OCRWorkflow</t>
+    <t>$model: MediaEngineBusinessProcessModel</t>
+  </si>
+  <si>
+    <t>com.armedia.acm.services.mediaengine.model.MediaEngineBusinessProcessModel</t>
+  </si>
+  <si>
+    <t>MediaEngineWorkFlow</t>
   </si>
 </sst>
 </file>
@@ -1091,8 +1091,8 @@
   </sheetPr>
   <dimension ref="A1:G18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1123,7 +1123,7 @@
         <v>0</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E2" s="1"/>
       <c r="F2" s="1"/>
@@ -1228,7 +1228,7 @@
       <c r="A12" s="2"/>
       <c r="B12" s="2"/>
       <c r="C12" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D12" s="3"/>
       <c r="E12" s="3"/>
@@ -1250,7 +1250,7 @@
       <c r="A14" s="2"/>
       <c r="B14" s="2"/>
       <c r="C14" s="5" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="D14" s="9"/>
       <c r="E14" s="9"/>
@@ -1276,7 +1276,7 @@
         <v>7</v>
       </c>
       <c r="C16" s="14" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D16" s="15" t="s">
         <v>8</v>
@@ -1288,7 +1288,7 @@
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="16"/>
       <c r="B17" s="17" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C17" s="18" t="s">
         <v>19</v>
@@ -1305,7 +1305,7 @@
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="16"/>
       <c r="B18" s="17" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C18" s="18" t="s">
         <v>20</v>

</xml_diff>